<commit_message>
updated current sense and zips
</commit_message>
<xml_diff>
--- a/Hardware/v3/current_sense_bom.xlsx
+++ b/Hardware/v3/current_sense_bom.xlsx
@@ -64,7 +64,7 @@
     <t xml:space="preserve">0402 Capacitor</t>
   </si>
   <si>
-    <t xml:space="preserve">445-5100-1-ND</t>
+    <t xml:space="preserve">445-1304-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">0.1uF</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">40F6015</t>
   </si>
   <si>
-    <t xml:space="preserve">MAX9923H</t>
+    <t xml:space="preserve">MAX9922</t>
   </si>
   <si>
     <t xml:space="preserve">UMAX10</t>
@@ -292,7 +292,7 @@
     <t xml:space="preserve">The MAX9922/MAX9923 ultra-precision, high-side current-</t>
   </si>
   <si>
-    <t xml:space="preserve">MAX9923HEUB+-ND</t>
+    <t xml:space="preserve">MAX9922EUB+TCT-ND </t>
   </si>
   <si>
     <t xml:space="preserve">LP3985</t>
@@ -394,12 +394,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -427,7 +431,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
+      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -472,497 +476,497 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="0" t="s">
+    <row r="2" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="F2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="0" t="s">
+      <c r="G2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" s="0" t="s">
+    <row r="3" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="0" t="s">
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="0" t="s">
+      <c r="F3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G3" s="0" t="s">
+      <c r="G3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+    <row r="4" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="F4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+    <row r="5" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="0" t="s">
+      <c r="E5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F5" s="0" t="s">
+      <c r="F5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="0" t="s">
+      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="H5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="n">
+    <row r="7" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="0" t="s">
+      <c r="F7" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="0" t="s">
+    <row r="8" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="n">
+    <row r="9" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="n">
         <v>0.04</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="n">
+    <row r="10" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="n">
         <v>0.12</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E10" s="0" t="s">
+      <c r="E10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="n">
+    <row r="11" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="n">
         <v>0.2</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="n">
+    <row r="12" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="n">
         <v>0.4</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E12" s="0" t="s">
+      <c r="E12" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2" t="n">
+    <row r="13" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="n">
         <v>1.2</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="0" t="s">
+      <c r="D13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="E13" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="n">
+    <row r="14" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="n">
         <v>12</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="0" t="s">
+      <c r="D14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="n">
+    <row r="15" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="n">
         <v>120</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="0" t="s">
+      <c r="D15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E15" s="0" t="s">
+      <c r="E15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B16" s="0" t="s">
+    <row r="16" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="0" t="s">
+      <c r="D16" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="0" t="s">
+      <c r="E16" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" s="0" t="s">
+    <row r="17" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="0" t="s">
+      <c r="D17" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="0" t="s">
+      <c r="E17" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="F17" s="0" t="s">
+      <c r="F17" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G17" s="0" t="s">
+      <c r="G17" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B18" s="0" t="s">
+    <row r="18" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D18" s="0" t="s">
+      <c r="D18" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="0" t="s">
+      <c r="E18" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="0" t="s">
+      <c r="F18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="G18" s="0" t="s">
+      <c r="G18" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B19" s="0" t="s">
+    <row r="19" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="0" t="s">
+      <c r="D19" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E19" s="0" t="s">
+      <c r="E19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="0" t="s">
+      <c r="F19" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G19" s="0" t="s">
+      <c r="G19" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
+    <row r="20" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B20" s="0" t="s">
+      <c r="B20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D20" s="0" t="s">
+      <c r="D20" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E20" s="0" t="s">
+      <c r="E20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="0" t="s">
+      <c r="F20" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="0" t="s">
+      <c r="G20" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B21" s="0" t="s">
+    <row r="21" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D21" s="0" t="s">
+      <c r="D21" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E21" s="0" t="s">
+      <c r="E21" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="F21" s="0" t="s">
+      <c r="F21" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I21" s="0" t="s">
+      <c r="I21" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B22" s="0" t="s">
+    <row r="22" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D22" s="0" t="s">
+      <c r="D22" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E22" s="0" t="s">
+      <c r="E22" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="F22" s="0" t="s">
+      <c r="F22" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="G22" s="0" t="s">
+      <c r="G22" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="B23" s="0" t="s">
+    <row r="23" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D23" s="0" t="s">
+      <c r="D23" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E23" s="0" t="s">
+      <c r="E23" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F23" s="0" t="s">
+      <c r="F23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G23" s="0" t="s">
+      <c r="G23" s="2" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>